<commit_message>
Change annuity of gas
</commit_message>
<xml_diff>
--- a/SeminarPaper/Model/input_data/tech.xlsx
+++ b/SeminarPaper/Model/input_data/tech.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Documents\GitHub\EnergyEconomics\SeminarPaper\Model\input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1511C5-238D-4866-B77E-C11BC182758D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D3D9E5-DACF-49DF-96C0-D4ED9830385A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="27">
   <si>
     <t>Type</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>PVRoof</t>
+  </si>
+  <si>
+    <t>MC[EUR/MWh_th]</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +428,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -597,7 +606,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -611,6 +620,20 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -966,15 +989,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
@@ -984,14 +1007,17 @@
     <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1000,13 +1026,13 @@
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -1015,13 +1041,13 @@
       <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -1030,17 +1056,20 @@
       <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1063,16 +1092,18 @@
         <v>45</v>
       </c>
       <c r="H2" s="3">
-        <v>89793.728510000001</v>
+        <f t="shared" ref="H2:H3" si="0">(((1+C12)^G2*C12)/((1+C12)^G2-1))*D2</f>
+        <v>89793.72850519084</v>
       </c>
       <c r="I2" s="3">
-        <v>139293.7285</v>
+        <f t="shared" ref="I2:I3" si="1">H2+F2</f>
+        <v>139293.72850519084</v>
       </c>
       <c r="J2" s="3">
         <v>0.36</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K8" si="0">J2/P2</f>
+        <f t="shared" ref="K2:K8" si="2">J2/Q2</f>
         <v>0.92307692307692302</v>
       </c>
       <c r="L2" s="3">
@@ -1081,19 +1112,23 @@
       <c r="M2" s="5">
         <v>6.03</v>
       </c>
-      <c r="N2">
-        <f>M2/P2</f>
+      <c r="N2" s="8">
+        <f t="shared" ref="N2:N8" si="3">M2/Q2</f>
         <v>15.461538461538462</v>
       </c>
-      <c r="O2" s="3">
-        <f t="shared" ref="O2:O8" si="1">(M2+(J2*L2))/(P2)</f>
+      <c r="O2">
+        <f>J2*L2+M2</f>
+        <v>20.43</v>
+      </c>
+      <c r="P2" s="7">
+        <f t="shared" ref="P2:P8" si="4">(M2+(J2*L2))/(Q2)</f>
         <v>52.38461538461538</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>0.39</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1116,16 +1151,18 @@
         <v>45</v>
       </c>
       <c r="H3" s="3">
-        <v>110104.2147</v>
+        <f t="shared" si="0"/>
+        <v>110104.21471469829</v>
       </c>
       <c r="I3" s="3">
-        <v>162104.21470000001</v>
+        <f t="shared" si="1"/>
+        <v>162104.21471469829</v>
       </c>
       <c r="J3" s="3">
         <v>0.35</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.84337349397590355</v>
       </c>
       <c r="L3" s="3">
@@ -1134,19 +1171,23 @@
       <c r="M3" s="5">
         <v>8.83</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N8" si="2">M3/P3</f>
+      <c r="N3" s="8">
+        <f t="shared" si="3"/>
         <v>21.277108433734941</v>
       </c>
-      <c r="O3" s="3">
-        <f t="shared" si="1"/>
+      <c r="O3">
+        <f t="shared" ref="O3:O8" si="5">J3*L3+M3</f>
+        <v>22.83</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="4"/>
         <v>55.012048192771083</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1166,19 +1207,21 @@
         <v>26500</v>
       </c>
       <c r="G4" s="3">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3">
-        <v>52210.889759999998</v>
+        <f>(((1+C14)^G4*C14)/((1+C14)^G4-1))*D4</f>
+        <v>60367.731754496665</v>
       </c>
       <c r="I4" s="3">
-        <v>78710.889760000005</v>
+        <f>H4+F4</f>
+        <v>86867.731754496665</v>
       </c>
       <c r="J4" s="3">
         <v>0.2</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.40404040404040409</v>
       </c>
       <c r="L4" s="3">
@@ -1187,19 +1230,23 @@
       <c r="M4" s="5">
         <v>28.69</v>
       </c>
-      <c r="N4">
-        <f t="shared" si="2"/>
+      <c r="N4" s="8">
+        <f t="shared" si="3"/>
         <v>57.959595959595966</v>
       </c>
-      <c r="O4" s="3">
-        <f t="shared" si="1"/>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>36.69</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="4"/>
         <v>74.12121212121211</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>0.495</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1222,16 +1269,18 @@
         <v>25</v>
       </c>
       <c r="H5" s="3">
-        <v>109834.4039</v>
+        <f t="shared" ref="H5:H8" si="6">(((1+C15)^G5*C15)/((1+C15)^G5-1))*D5</f>
+        <v>109834.40389920746</v>
       </c>
       <c r="I5" s="3">
-        <v>122834.4039</v>
+        <f t="shared" ref="I5:I8" si="7">H5+F5</f>
+        <v>122834.40389920746</v>
       </c>
       <c r="J5" s="3">
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="3">
@@ -1240,19 +1289,23 @@
       <c r="M5" s="6">
         <v>0</v>
       </c>
-      <c r="N5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="1"/>
+      <c r="N5" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P5" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1275,16 +1328,18 @@
         <v>25</v>
       </c>
       <c r="H6" s="3">
-        <v>175465.42689999999</v>
+        <f t="shared" si="6"/>
+        <v>175465.42690099485</v>
       </c>
       <c r="I6" s="3">
-        <v>268465.42690000002</v>
+        <f t="shared" si="7"/>
+        <v>268465.42690099485</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="3">
@@ -1294,18 +1349,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P6" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1328,16 +1387,18 @@
         <v>25</v>
       </c>
       <c r="H7" s="3">
-        <v>54917.201950000002</v>
+        <f t="shared" si="6"/>
+        <v>54917.201949603732</v>
       </c>
       <c r="I7" s="3">
-        <v>69917.201950000002</v>
+        <f t="shared" si="7"/>
+        <v>69917.201949603739</v>
       </c>
       <c r="J7" s="3">
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L7" s="3">
@@ -1347,18 +1408,22 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1381,16 +1446,18 @@
         <v>25</v>
       </c>
       <c r="H8" s="3">
-        <v>68965.788490000006</v>
+        <f t="shared" si="6"/>
+        <v>68965.788494851193</v>
       </c>
       <c r="I8" s="3">
-        <v>85965.788490000006</v>
+        <f t="shared" si="7"/>
+        <v>85965.788494851193</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L8" s="3">
@@ -1400,18 +1467,22 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P8" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1427,10 +1498,10 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -1439,22 +1510,22 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>0.05</v>
       </c>

</xml_diff>